<commit_message>
create all tables for devices
</commit_message>
<xml_diff>
--- a/notebook.xlsx
+++ b/notebook.xlsx
@@ -4,18 +4,17 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="105" windowWidth="15120" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="105" windowWidth="15120" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="Apple" sheetId="1" r:id="rId1"/>
-    <sheet name="Samsung" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Модель</t>
   </si>
@@ -23,19 +22,13 @@
     <t>Стоимость</t>
   </si>
   <si>
-    <t>Samsung Galaxy Watch5</t>
+    <t>Macbook Pro 13</t>
   </si>
   <si>
-    <t>Samsung Galaxy Watch4</t>
+    <t>Macbook Pro 14</t>
   </si>
   <si>
-    <t>Apple Watch Ultra, 49mm</t>
-  </si>
-  <si>
-    <t>Apple Watch Series 8, 41mm</t>
-  </si>
-  <si>
-    <t>Apple Watch Series 8, 45mm</t>
+    <t>Macbook Pro 15</t>
   </si>
 </sst>
 </file>
@@ -87,7 +80,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -138,27 +131,81 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -453,96 +500,55 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="66" style="2" customWidth="1"/>
-    <col min="2" max="2" width="20.42578125" style="5" customWidth="1"/>
+    <col min="1" max="1" width="66" style="1" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="16.5" thickBot="1">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
+      <c r="A2" s="8" t="s">
+        <v>2</v>
       </c>
       <c r="B2" s="4">
-        <v>100000</v>
+        <v>45000</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="1" t="s">
-        <v>5</v>
+      <c r="A3" s="9" t="s">
+        <v>3</v>
       </c>
       <c r="B3" s="5">
         <v>40000</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="1" t="s">
-        <v>6</v>
+      <c r="A4" s="9" t="s">
+        <v>4</v>
       </c>
       <c r="B4" s="5">
         <v>50000</v>
       </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="180" verticalDpi="180" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="55" style="5" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" style="5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="15.75">
-      <c r="A1" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="5">
-        <v>15000</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="5">
-        <v>17000</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
fix some problems with other devices
</commit_message>
<xml_diff>
--- a/notebook.xlsx
+++ b/notebook.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Модель</t>
   </si>
@@ -29,6 +29,21 @@
   </si>
   <si>
     <t>Macbook Pro 15</t>
+  </si>
+  <si>
+    <t>Macbook Pro 16</t>
+  </si>
+  <si>
+    <t>Macbook Air 13</t>
+  </si>
+  <si>
+    <t>Macbook Air 11</t>
+  </si>
+  <si>
+    <t>Macbook Air M1</t>
+  </si>
+  <si>
+    <t>Macbook Air M2</t>
   </si>
 </sst>
 </file>
@@ -48,28 +63,25 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <name val="JetBrains Mono"/>
-      <family val="3"/>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
       <charset val="204"/>
     </font>
     <font>
-      <b/>
+      <sz val="12"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <charset val="204"/>
+    </font>
+    <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
       <charset val="204"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -80,7 +92,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -159,19 +171,6 @@
       <left style="medium">
         <color auto="1"/>
       </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
       <right style="thin">
         <color auto="1"/>
       </right>
@@ -187,25 +186,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -500,10 +500,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -513,39 +513,76 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="16.5" thickBot="1">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="8" t="s">
+    <row r="2" spans="1:2" ht="15.75">
+      <c r="A2" s="9" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="4">
         <v>45000</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="9" t="s">
+    <row r="3" spans="1:2" ht="15.75">
+      <c r="A3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="6">
         <v>40000</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="9" t="s">
+    <row r="4" spans="1:2" ht="15.75">
+      <c r="A4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="6">
         <v>50000</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="6"/>
+    <row r="5" spans="1:2" ht="15.75">
+      <c r="A5" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="6">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15.75">
+      <c r="A6" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="6">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15.75">
+      <c r="A7" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="6">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15.75">
+      <c r="A8" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="6">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="15.75">
+      <c r="A9" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="6">
+        <v>50000</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>